<commit_message>
Added skos definition for A320
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -1,17 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/horridge/IdeaProjects/Excel2SKOS-Examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50124A3F-639A-1646-AB51-6DF4388AD001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -27,13 +46,20 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Arial"/>
       </rPr>
       <t>http://protege.stanford</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>.edu/thesauri/aero/</t>
     </r>
   </si>
@@ -87,37 +113,64 @@
   </si>
   <si>
     <t>A380</t>
+  </si>
+  <si>
+    <t>A320 Family Aircraft.  An A320 is a narrow body twin jet aircraft that is manufactured by Airbus</t>
+  </si>
+  <si>
+    <t>skos:definition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,49 +178,57 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -357,25 +418,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.75"/>
-    <col customWidth="1" min="3" max="3" width="15.88"/>
-    <col customWidth="1" min="4" max="4" width="19.25"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -383,12 +450,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -399,7 +466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -407,7 +474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -415,7 +482,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -428,137 +495,143 @@
       <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="E7" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="str">
-        <f t="shared" ref="A8:A16" si="1">"aero:" &amp; B8</f>
+        <f t="shared" ref="A8:A16" si="0">"aero:" &amp; B8</f>
         <v>aero:A300</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="6" t="str">
-        <f t="shared" ref="C8:C16" si="2">"Airbus " &amp; B8</f>
+        <f t="shared" ref="C8:C16" si="1">"Airbus " &amp; B8</f>
         <v>Airbus A300</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>aero:A310</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Airbus A310</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>aero:A320</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Airbus A320</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="E10" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>aero:A320-100</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Airbus A320-100</v>
       </c>
       <c r="D11" s="6" t="str">
-        <f t="shared" ref="D11:D12" si="3">$A$10</f>
+        <f t="shared" ref="D11:D12" si="2">$A$10</f>
         <v>aero:A320</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>aero:A320-200</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Airbus A320-200</v>
+      </c>
+      <c r="D12" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>Airbus A320-200</v>
-      </c>
-      <c r="D12" s="6" t="str">
-        <f t="shared" si="3"/>
         <v>aero:A320</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>aero:A330</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Airbus A330</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>aero:A340</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Airbus A340</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>aero:A350</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Airbus A350</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>aero:A380</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Airbus A380</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B1"/>
-    <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>